<commit_message>
Repo cleanup before site publish.
outlet menus need link updates + engine implementation.
</commit_message>
<xml_diff>
--- a/files/menus/green_mountain/pokebowls_greenmountain.xlsx
+++ b/files/menus/green_mountain/pokebowls_greenmountain.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ajaxproto\files\menus\green_mountain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96C2C751-6B90-468E-9D52-E3017D03AEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08E95D2E-1DF1-4191-A42B-3797689B344D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6855" windowWidth="29040" windowHeight="15840" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
+    <workbookView xWindow="4725" yWindow="6270" windowWidth="27405" windowHeight="14325" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
   </bookViews>
   <sheets>
-    <sheet name="salads_greenmountain" sheetId="1" r:id="rId1"/>
+    <sheet name="pokebowls_greenmountain" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Ingredients</t>
   </si>
@@ -56,55 +56,58 @@
     <t>NA</t>
   </si>
   <si>
+    <t>Egg, Sausage</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>VGN, GF, DF</t>
+  </si>
+  <si>
+    <t>Turkey / Bacon / Cheddar Cheese / Lettuce / Tomato / Garlic Aioli</t>
+  </si>
+  <si>
+    <t>Turkey / Swiss Cheese / Roasted Onion / Tomato / Cucumber / Mixed Greens / Spicy Mayo</t>
+  </si>
+  <si>
+    <t>Allergens</t>
+  </si>
+  <si>
+    <t>Wheat, sulphites, egg.</t>
+  </si>
+  <si>
+    <t>No known priority allergens</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>GF,VEG</t>
+  </si>
+  <si>
+    <t>Aloha</t>
+  </si>
+  <si>
+    <t>Coastal</t>
+  </si>
+  <si>
+    <t>Tuna</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Veggie</t>
+  </si>
+  <si>
+    <t>Smoked salmon / yellowfin tuna / cucumber / carrot / pineapple / guacamole / spicy mayo / green onion / unagi sauce / sesame seeds</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
     <t>waffles</t>
-  </si>
-  <si>
-    <t>Egg, Sausage</t>
-  </si>
-  <si>
-    <t>Potato</t>
-  </si>
-  <si>
-    <t>VGN, GF, DF</t>
-  </si>
-  <si>
-    <t>Turkey / Bacon / Cheddar Cheese / Lettuce / Tomato / Garlic Aioli</t>
-  </si>
-  <si>
-    <t>Turkey / Swiss Cheese / Roasted Onion / Tomato / Cucumber / Mixed Greens / Spicy Mayo</t>
-  </si>
-  <si>
-    <t>Allergens</t>
-  </si>
-  <si>
-    <t>Wheat, sulphites, egg.</t>
-  </si>
-  <si>
-    <t>No known priority allergens</t>
-  </si>
-  <si>
-    <t>GF</t>
-  </si>
-  <si>
-    <t>GF,VEG</t>
-  </si>
-  <si>
-    <t>Aloha</t>
-  </si>
-  <si>
-    <t>Coastal</t>
-  </si>
-  <si>
-    <t>Tuna</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Veggie</t>
-  </si>
-  <si>
-    <t>Smoked salmon / yellowfin tuna / cucumber / carrot / pineapple / guacamole / spicy mayo / green onion / unagi sauce / sesame seeds</t>
   </si>
 </sst>
 </file>
@@ -146,11 +149,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,17 +169,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}" name="Table3" displayName="Table3" ref="A1:F6" totalsRowShown="0">
-  <autoFilter ref="A1:F6" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}" name="Table3" displayName="Table3" ref="A1:G6" totalsRowShown="0">
+  <autoFilter ref="A1:G6" xr:uid="{A32FF9D1-238C-44C9-AD02-5D859735230E}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AA44CCDF-F9E2-4FB6-9AED-85FE3A3C6008}" name="ItemName"/>
     <tableColumn id="2" xr3:uid="{9D7FC130-DF66-4465-8F0B-6015043C6AA1}" name="Ingredients"/>
     <tableColumn id="7" xr3:uid="{364DC3EB-6DF2-4CD4-84D8-820702E66F1F}" name="Allergens"/>
     <tableColumn id="3" xr3:uid="{9F2485F9-EFCE-415F-9AF4-2B5A16080CD5}" name="LocalIngredients"/>
     <tableColumn id="4" xr3:uid="{11D88A0B-C840-4F23-81DF-C249BC9C7872}" name="Diet"/>
     <tableColumn id="5" xr3:uid="{378390CC-E66E-4719-939E-E825F4A2EB3E}" name="nutritionLabel"/>
+    <tableColumn id="6" xr3:uid="{23E938A5-A80A-4A49-8C04-E8A657333980}" name="Column1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -480,13 +481,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4FEC9-4E15-443B-89A8-5C76E19963E8}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
@@ -496,7 +497,7 @@
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -504,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -515,102 +516,108 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
+      <c r="F3" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>